<commit_message>
MUDANCA NA TABELA XLX
</commit_message>
<xml_diff>
--- a/Projeto/Tabela_DFA.xlsx
+++ b/Projeto/Tabela_DFA.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -866,7 +866,7 @@
         <v>5</v>
       </c>
       <c r="M7" t="str">
-        <v>14</v>
+        <v>6.5</v>
       </c>
       <c r="N7" t="str">
         <v>5</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Menor(7)</v>
+        <v>/(6.5)</v>
       </c>
       <c r="B8" t="str">
         <v>14</v>
@@ -910,58 +910,58 @@
         <v>14</v>
       </c>
       <c r="D8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N8" t="str">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T8" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U8" t="str">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="V8" t="str">
         <v>14</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Maior(8)</v>
+        <v>Menor(7)</v>
       </c>
       <c r="B9" t="str">
         <v>14</v>
@@ -1011,7 +1011,7 @@
         <v>15</v>
       </c>
       <c r="N9" t="str">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O9" t="str">
         <v>15</v>
@@ -1032,7 +1032,7 @@
         <v>15</v>
       </c>
       <c r="U9" t="str">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V9" t="str">
         <v>14</v>
@@ -1043,13 +1043,13 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Diferente(9)</v>
+        <v>Maior(8)</v>
       </c>
       <c r="B10" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" t="str">
         <v>15</v>
@@ -1082,7 +1082,7 @@
         <v>15</v>
       </c>
       <c r="N10" t="str">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O10" t="str">
         <v>15</v>
@@ -1103,10 +1103,10 @@
         <v>15</v>
       </c>
       <c r="U10" t="str">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V10" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W10" t="str">
         <v>não</v>
@@ -1114,13 +1114,13 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Atribuicao(10)</v>
+        <v>Diferente(9)</v>
       </c>
       <c r="B11" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D11" t="str">
         <v>15</v>
@@ -1153,7 +1153,7 @@
         <v>15</v>
       </c>
       <c r="N11" t="str">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="O11" t="str">
         <v>15</v>
@@ -1174,10 +1174,10 @@
         <v>15</v>
       </c>
       <c r="U11" t="str">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="V11" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="W11" t="str">
         <v>não</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Comparacao(11)</v>
+        <v>Atribuicao(10)</v>
       </c>
       <c r="B12" t="str">
         <v>14</v>
@@ -1194,55 +1194,55 @@
         <v>14</v>
       </c>
       <c r="D12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N12" t="str">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="T12" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="U12" t="str">
         <v>14</v>
@@ -1256,67 +1256,67 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>MaiorIgual(12)</v>
+        <v>Comparacao(11)</v>
       </c>
       <c r="B13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="str">
         <v>14</v>
       </c>
       <c r="D13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T13" t="str">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U13" t="str">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="V13" t="str">
         <v>14</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>MenorIgual(13)</v>
+        <v>MaiorIgual(12)</v>
       </c>
       <c r="B14" t="str">
         <v>15</v>
@@ -1387,7 +1387,7 @@
         <v>15</v>
       </c>
       <c r="U14" t="str">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V14" t="str">
         <v>14</v>
@@ -1398,10 +1398,10 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>+-*/ (13.5)</v>
+        <v>MenorIgual(13)</v>
       </c>
       <c r="B15" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" t="str">
         <v>14</v>
@@ -1431,7 +1431,7 @@
         <v>15</v>
       </c>
       <c r="L15" t="str">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M15" t="str">
         <v>15</v>
@@ -1458,31 +1458,102 @@
         <v>15</v>
       </c>
       <c r="U15" t="str">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V15" t="str">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="W15" t="str">
+        <v>não</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Fim(14)</v>
-      </c>
-      <c r="W16" t="str">
-        <v>sim</v>
+        <v>+-*/ (13.5)</v>
+      </c>
+      <c r="B16" t="str">
+        <v>14</v>
+      </c>
+      <c r="C16" t="str">
+        <v>14</v>
+      </c>
+      <c r="D16" t="str">
+        <v>15</v>
+      </c>
+      <c r="E16" t="str">
+        <v>15</v>
+      </c>
+      <c r="F16" t="str">
+        <v>15</v>
+      </c>
+      <c r="G16" t="str">
+        <v>15</v>
+      </c>
+      <c r="H16" t="str">
+        <v>15</v>
+      </c>
+      <c r="I16" t="str">
+        <v>15</v>
+      </c>
+      <c r="J16" t="str">
+        <v>15</v>
+      </c>
+      <c r="K16" t="str">
+        <v>15</v>
+      </c>
+      <c r="L16" t="str">
+        <v>14</v>
+      </c>
+      <c r="M16" t="str">
+        <v>15</v>
+      </c>
+      <c r="N16" t="str">
+        <v>15</v>
+      </c>
+      <c r="O16" t="str">
+        <v>15</v>
+      </c>
+      <c r="P16" t="str">
+        <v>15</v>
+      </c>
+      <c r="Q16" t="str">
+        <v>15</v>
+      </c>
+      <c r="R16" t="str">
+        <v>15</v>
+      </c>
+      <c r="S16" t="str">
+        <v>15</v>
+      </c>
+      <c r="T16" t="str">
+        <v>15</v>
+      </c>
+      <c r="U16" t="str">
+        <v>14</v>
+      </c>
+      <c r="V16" t="str">
+        <v>15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
+        <v>Fim(14)</v>
+      </c>
+      <c r="W17" t="str">
+        <v>sim</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
         <v>Erro(15)</v>
       </c>
-      <c r="W17" t="str">
+      <c r="W18" t="str">
         <v>não</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:W17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:W18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>